<commit_message>
update maket.xlsx 10.12.22 1:09
</commit_message>
<xml_diff>
--- a/maket.xlsx
+++ b/maket.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdgbi\Desktop\S\Vision\predvidenie_vision\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA8F6F3-04CD-4D5D-9959-FCD17FB31AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4DCC6B27-57E4-48D8-B6D7-57E28F728DE8}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="482" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="главная страница" sheetId="1" r:id="rId1"/>
     <sheet name="состояние в настоящий момент" sheetId="2" r:id="rId2"/>
+    <sheet name="возможное состояние" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="98">
   <si>
     <t>Возможное состояние</t>
   </si>
@@ -206,12 +201,126 @@
   </si>
   <si>
     <t>Состояние в настоящий момент</t>
+  </si>
+  <si>
+    <t>убеждения</t>
+  </si>
+  <si>
+    <t>Наши реакции соответствуют нашим внутренним картам.</t>
+  </si>
+  <si>
+    <t>""Карта" - не "территория"". ("меню-не пища").</t>
+  </si>
+  <si>
+    <t>Значение зависит от контекста.</t>
+  </si>
+  <si>
+    <t>Разум и тело неизбежно влияют друг на друга.</t>
+  </si>
+  <si>
+    <t>Индвивидуальные навыки являются результатом совершенствования и установления последовательности использования репрезентативных систем.</t>
+  </si>
+  <si>
+    <t>Мы уважаем модели мира других людей.</t>
+  </si>
+  <si>
+    <t>страхи</t>
+  </si>
+  <si>
+    <t>Если есть конфеты, то будет больно.</t>
+  </si>
+  <si>
+    <t>желания</t>
+  </si>
+  <si>
+    <t>Личность и поведение - это различные явления. Мы представляем собой нечто большее, чем наше поведение.</t>
+  </si>
+  <si>
+    <t>Каждый вид поведения практичен и полезен в опреденном контексте.</t>
+  </si>
+  <si>
+    <t>Мы оцениваем поведение и изменения в терминах контекста и экологии.</t>
+  </si>
+  <si>
+    <t>Мы не можем не общаться.</t>
+  </si>
+  <si>
+    <t>Способ коммуникации влияет на наше восприятие.</t>
+  </si>
+  <si>
+    <t>Смысл коммуникации заключается в той реакции, которую она вызывает.</t>
+  </si>
+  <si>
+    <t>Человек, задающий фрейм коммуникации, контролирует её.</t>
+  </si>
+  <si>
+    <t>"Не бывает поражений, есть только обратная связь".</t>
+  </si>
+  <si>
+    <t>Человек, обладающий наибольшей гибкостью, имеет наибольшее влияние в системе.</t>
+  </si>
+  <si>
+    <t>Сопротивление указывает на отсутствие раппорта.</t>
+  </si>
+  <si>
+    <t>Мы обладаем необходимыми для достижения цели внутренними ресурсами.</t>
+  </si>
+  <si>
+    <t>Мы способны научиться чему-либо с одной попытки.</t>
+  </si>
+  <si>
+    <t>Любая коммуникация должна увеличивать количество доступных альтернатив.</t>
+  </si>
+  <si>
+    <t>Совершая какой-либо поступок, мы выбираем наилучший из имеющихся у нас в данный момент вариантов.</t>
+  </si>
+  <si>
+    <t>Мы можем управлять своим мозгом и контролировать результаты.</t>
+  </si>
+  <si>
+    <t>интеллект</t>
+  </si>
+  <si>
+    <t>Общественное должно быть лучше индивидуального.</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Есть Единый Бог Отец, Вседержитель, Творец Небу и Земли…</t>
+  </si>
+  <si>
+    <t>Сотворять кумира нельзя.</t>
+  </si>
+  <si>
+    <t>Произносить имя Господа, Бога нельзя.</t>
+  </si>
+  <si>
+    <t>Нужно работать 6 дней, а в субботу отдыхать.</t>
+  </si>
+  <si>
+    <t>Нужно почитать отца и мать.</t>
+  </si>
+  <si>
+    <t>Нельзя убивать.</t>
+  </si>
+  <si>
+    <t>Нельзя прелюбодействовать.</t>
+  </si>
+  <si>
+    <t>Нельзя красть.</t>
+  </si>
+  <si>
+    <t>Нельзя желать чужую жену. Нельзя желать чужого дома. Нельзя желать чужую землю. Нельзя желать чужих животных. Нельзя желать ничего чужого.</t>
+  </si>
+  <si>
+    <t>Нельзя лгать.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,10 +370,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -572,40 +686,40 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9A18F8-59D2-4F82-BBC3-EC5E934915DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -622,7 +736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>3</v>
       </c>
@@ -630,7 +744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>5</v>
       </c>
@@ -644,26 +758,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6418321B-0D1F-4FDC-B82B-CB08C288AB04}">
-  <dimension ref="A1:C50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -671,252 +785,476 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B48" s="2" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B66" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B73" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B78" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B82" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B48" r:id="rId1" xr:uid="{CF8962E1-26C4-4282-9ECF-CA46CB3472C0}"/>
+    <hyperlink ref="B49" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated maket.xlsx 12.12.2022 16:26
</commit_message>
<xml_diff>
--- a/maket.xlsx
+++ b/maket.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdgbi\Desktop\S\Vision\predvidenie_vision\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68181C4B-F134-4FBB-90AD-7FF7F313F49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="482" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="482" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="главная страница" sheetId="1" r:id="rId1"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
   <si>
     <t>Возможное состояние</t>
   </si>
@@ -315,12 +321,18 @@
   </si>
   <si>
     <t>Нельзя лгать.</t>
+  </si>
+  <si>
+    <t>еда</t>
+  </si>
+  <si>
+    <t>здоровье</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -686,40 +698,40 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -736,7 +748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>3</v>
       </c>
@@ -744,7 +756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>5</v>
       </c>
@@ -758,26 +770,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C89"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -785,7 +797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -793,7 +805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -801,444 +813,454 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B72" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B82" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B83" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B86" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B49" r:id="rId1"/>
+    <hyperlink ref="B49" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1246,14 +1268,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>